<commit_message>
analise preditiva para produção e demanda dos items da cesta básica
calculo das media moveis para projeção da produçao dos items da cesta básica
</commit_message>
<xml_diff>
--- a/df_arroz.xlsx
+++ b/df_arroz.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dcc-fellowship-ciencia-de-dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B627A5D-C2D8-437D-B349-1E0F15B40189}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA3D332-A67F-44FA-9294-A61AF941AB88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -460,7 +460,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
calculo das médias moveis
</commit_message>
<xml_diff>
--- a/df_arroz.xlsx
+++ b/df_arroz.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dcc-fellowship-ciencia-de-dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA3D332-A67F-44FA-9294-A61AF941AB88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A92312B5-A4EE-4848-9AC8-4703FDA9D929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -104,7 +104,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -119,6 +119,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -460,7 +463,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,13 +491,13 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+      <c r="A2" s="4">
         <v>2018</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="2">
+      <c r="B2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="6">
         <v>11808412</v>
       </c>
       <c r="D2" s="5">
@@ -503,13 +506,13 @@
       <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="A3" s="4">
         <v>2019</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="2">
+      <c r="B3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="6">
         <v>10368639</v>
       </c>
       <c r="D3">
@@ -518,13 +521,13 @@
       <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="A4" s="4">
         <v>2020</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="2">
+      <c r="B4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="6">
         <v>11091011</v>
       </c>
       <c r="D4">
@@ -533,14 +536,14 @@
       <c r="E4" s="4"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+      <c r="A5" s="4">
         <v>2021</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="2">
-        <v>11533391</v>
+      <c r="B5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="6">
+        <v>11533393</v>
       </c>
       <c r="D5">
         <v>4368745.2467200002</v>
@@ -548,14 +551,14 @@
       <c r="E5" s="4"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+      <c r="A6" s="4">
         <v>2022</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="4">
-        <v>11405422.666666666</v>
+      <c r="B6" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="6">
+        <v>11405425</v>
       </c>
       <c r="D6">
         <v>4399688.4991999995</v>
@@ -563,14 +566,14 @@
       <c r="E6" s="4"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+      <c r="A7" s="4">
         <v>2023</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="4">
-        <v>11535961.611111112</v>
+      <c r="B7" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="6">
+        <v>11535964.333333334</v>
       </c>
       <c r="D7">
         <v>4429501.8291199999</v>
@@ -578,14 +581,14 @@
       <c r="E7" s="4"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+      <c r="A8" s="4">
         <v>2024</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="4">
-        <v>11381160.879629629</v>
+      <c r="B8" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="6">
+        <v>11381164.055555554</v>
       </c>
       <c r="D8">
         <v>4458177.7817600006</v>
@@ -593,14 +596,14 @@
       <c r="E8" s="4"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+      <c r="A9" s="4">
         <v>2025</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="4">
-        <v>11309952.359567901</v>
+      <c r="B9" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="6">
+        <v>11309956.064814815</v>
       </c>
       <c r="D9">
         <v>4485715.8246400002</v>
@@ -608,56 +611,56 @@
       <c r="E9" s="4"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
+      <c r="A10" s="4">
         <v>2026</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="4">
-        <v>11466837.919495882</v>
+      <c r="B10" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="6">
+        <v>11466842.24228395</v>
       </c>
       <c r="D10">
         <v>4512082.5343999993</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
+      <c r="A11" s="4">
         <v>2027</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="4">
-        <v>11529475.739411866</v>
+      <c r="B11" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="6">
+        <v>11529480.78266461</v>
       </c>
       <c r="D11">
         <v>4537246.3923199996</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
+      <c r="A12" s="4">
         <v>2028</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" s="4">
-        <v>11528823.19598051</v>
+      <c r="B12" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="6">
+        <v>11528828.746442042</v>
       </c>
       <c r="D12">
         <v>4561175.9411199996</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
+      <c r="A13" s="4">
         <v>2029</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" s="4">
-        <v>11549389.95086615</v>
+      <c r="B13" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="6">
+        <v>11549396.037515717</v>
       </c>
       <c r="D13">
         <v>4583860.3263999997</v>
@@ -665,14 +668,14 @@
       <c r="G13" s="4"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
+      <c r="A14" s="4">
         <v>2030</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" s="4">
-        <v>11551628.007491991</v>
+      <c r="B14" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="6">
+        <v>11551634.654879449</v>
       </c>
       <c r="D14">
         <v>4605306.10176</v>

</xml_diff>